<commit_message>
completed 4th testcase successfully
</commit_message>
<xml_diff>
--- a/Testcases.xlsx
+++ b/Testcases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work Docs\E-Commerce Project Guru99\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sushmitha\Magento-E-commerce-Website-automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D417000-7E71-43FF-AF39-9B31F50DF25E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5CF9B2D-DFF8-4E07-83D7-8A3B1FE3027A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{623458BB-9245-4834-9240-71D9B0327D92}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{623458BB-9245-4834-9240-71D9B0327D92}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Verify item in Mobile List page can be sorted by 'Name'</t>
   </si>
@@ -94,6 +94,25 @@
   </si>
   <si>
     <t>Verify that you cannot add more product in cart than the product available in store</t>
+  </si>
+  <si>
+    <t>Verify that you are able to compare two product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.A Popup window opens with headind as 'COMPARE PRODUCTS' and the selected products are present in it. 
+2. Popup window is closed </t>
+  </si>
+  <si>
+    <t>Phone 1 Sony Xperia
+Phone 2 IPHONE</t>
+  </si>
+  <si>
+    <t>1. Goto http://live.techpanda.org/ 
+2.Click on 'MOBILE' menu 
+3.In mobile products list , click on 'Add To Compare' for 2 mobiles
+ 4 Click on 'COMPARE' button.
+5. Verify the pop-up window and check that the products are reflected in it 
+6 Close the Popup Windows</t>
   </si>
 </sst>
 </file>
@@ -129,13 +148,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -451,23 +476,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C55CBE53-C99B-4700-908D-B54CD309EFAA}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="71" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="67.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7265625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="58.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="2" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="75.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="72.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="58.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
@@ -481,49 +506,67 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="3" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>